<commit_message>
public to private modified
</commit_message>
<xml_diff>
--- a/MakeMyTripBus/TestData/InputData.xlsx
+++ b/MakeMyTripBus/TestData/InputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\249079\source\repos\Selenium_MiniProject\MakeMyTripBus\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408E3823-A060-402F-A7B9-CD6B3D0B1A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1B8A89-1165-402B-A729-FC8108890699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,7 +432,7 @@
         <v>14</v>
       </c>
       <c r="H2">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>